<commit_message>
move disabled and autoselect next based on pp
</commit_message>
<xml_diff>
--- a/moves.xlsx
+++ b/moves.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="207">
   <si>
     <t>Bug Bite</t>
   </si>
@@ -632,6 +632,9 @@
   </si>
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t>pp1</t>
   </si>
 </sst>
 </file>
@@ -967,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E184"/>
+  <dimension ref="A1:F184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,7 +985,7 @@
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>201</v>
       </c>
@@ -993,13 +996,16 @@
         <v>203</v>
       </c>
       <c r="D1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="E1" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1010,13 +1016,17 @@
         <v>100</v>
       </c>
       <c r="D2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>ROUND(D2,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1027,13 +1037,17 @@
         <v>100</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="0">ROUND(D3,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1044,13 +1058,17 @@
         <v>95</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1061,13 +1079,17 @@
         <v>100</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1078,13 +1100,17 @@
         <v>85</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1095,13 +1121,17 @@
         <v>95</v>
       </c>
       <c r="D7">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1112,13 +1142,17 @@
         <v>100</v>
       </c>
       <c r="D8">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1129,13 +1163,17 @@
         <v>100</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1146,13 +1184,17 @@
         <v>95</v>
       </c>
       <c r="D10">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1163,13 +1205,17 @@
         <v>100</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1180,13 +1226,17 @@
         <v>100</v>
       </c>
       <c r="D12">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1197,13 +1247,17 @@
         <v>100</v>
       </c>
       <c r="D13">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1214,13 +1268,17 @@
         <v>100</v>
       </c>
       <c r="D14">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E14" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1231,13 +1289,17 @@
         <v>100</v>
       </c>
       <c r="D15">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1248,13 +1310,17 @@
         <v>100</v>
       </c>
       <c r="D16">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1265,13 +1331,17 @@
         <v>100</v>
       </c>
       <c r="D17">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1282,13 +1352,17 @@
         <v>100</v>
       </c>
       <c r="D18">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1299,13 +1373,17 @@
         <v>100</v>
       </c>
       <c r="D19">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E19" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1316,13 +1394,17 @@
         <v>100</v>
       </c>
       <c r="D20">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E20" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1333,13 +1415,17 @@
         <v>100</v>
       </c>
       <c r="D21">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1350,13 +1436,17 @@
         <v>100</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E22" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1367,13 +1457,17 @@
         <v>100</v>
       </c>
       <c r="D23">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="E23" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1384,13 +1478,17 @@
         <v>100</v>
       </c>
       <c r="D24">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1401,13 +1499,17 @@
         <v>100</v>
       </c>
       <c r="D25">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E25" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1418,13 +1520,17 @@
         <v>100</v>
       </c>
       <c r="D26">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E26" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1435,13 +1541,17 @@
         <v>100</v>
       </c>
       <c r="D27">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1452,13 +1562,17 @@
         <v>100</v>
       </c>
       <c r="D28">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E28" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1469,13 +1583,17 @@
         <v>100</v>
       </c>
       <c r="D29">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E29" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1486,13 +1604,17 @@
         <v>100</v>
       </c>
       <c r="D30">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E30" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1503,13 +1625,17 @@
         <v>90</v>
       </c>
       <c r="D31">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E31" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1520,13 +1646,17 @@
         <v>100</v>
       </c>
       <c r="D32">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E32" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1537,13 +1667,17 @@
         <v>75</v>
       </c>
       <c r="D33">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E33" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1554,13 +1688,17 @@
         <v>90</v>
       </c>
       <c r="D34">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E34" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1571,13 +1709,17 @@
         <v>100</v>
       </c>
       <c r="D35">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E35" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1588,13 +1730,17 @@
         <v>100</v>
       </c>
       <c r="D36">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E36" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1605,13 +1751,17 @@
         <v>100</v>
       </c>
       <c r="D37">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E37" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -1622,13 +1772,17 @@
         <v>70</v>
       </c>
       <c r="D38">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -1639,13 +1793,17 @@
         <v>95</v>
       </c>
       <c r="D39">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E39" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -1656,13 +1814,17 @@
         <v>100</v>
       </c>
       <c r="D40">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E40" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -1673,13 +1835,17 @@
         <v>90</v>
       </c>
       <c r="D41">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E41" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -1690,13 +1856,17 @@
         <v>100</v>
       </c>
       <c r="D42">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E42" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -1707,13 +1877,17 @@
         <v>100</v>
       </c>
       <c r="D43">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E43" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -1724,13 +1898,17 @@
         <v>50</v>
       </c>
       <c r="D44">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E44" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -1741,13 +1919,17 @@
         <v>100</v>
       </c>
       <c r="D45">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E45" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -1758,13 +1940,17 @@
         <v>100</v>
       </c>
       <c r="D46">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E46" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -1775,13 +1961,17 @@
         <v>75</v>
       </c>
       <c r="D47">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E47" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -1792,13 +1982,17 @@
         <v>100</v>
       </c>
       <c r="D48">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E48" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -1809,13 +2003,17 @@
         <v>100</v>
       </c>
       <c r="D49">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -1826,13 +2024,17 @@
         <v>100</v>
       </c>
       <c r="D50">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E50" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -1843,13 +2045,17 @@
         <v>90</v>
       </c>
       <c r="D51">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E51" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -1860,13 +2066,17 @@
         <v>100</v>
       </c>
       <c r="D52">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E52" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -1877,13 +2087,17 @@
         <v>100</v>
       </c>
       <c r="D53">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E53" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -1894,13 +2108,17 @@
         <v>100</v>
       </c>
       <c r="D54">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E54" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -1911,13 +2129,17 @@
         <v>100</v>
       </c>
       <c r="D55">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E55" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -1928,13 +2150,17 @@
         <v>100</v>
       </c>
       <c r="D56">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E56" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -1945,13 +2171,17 @@
         <v>100</v>
       </c>
       <c r="D57">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E57" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>62</v>
       </c>
@@ -1962,13 +2192,17 @@
         <v>80</v>
       </c>
       <c r="D58">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E58" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -1979,13 +2213,17 @@
         <v>100</v>
       </c>
       <c r="D59">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E59" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -1996,13 +2234,17 @@
         <v>50</v>
       </c>
       <c r="D60">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E60" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -2013,13 +2255,17 @@
         <v>100</v>
       </c>
       <c r="D61">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="E61" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>66</v>
       </c>
@@ -2030,13 +2276,17 @@
         <v>100</v>
       </c>
       <c r="D62">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E62" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -2047,13 +2297,17 @@
         <v>90</v>
       </c>
       <c r="D63">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E63" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -2064,13 +2318,17 @@
         <v>100</v>
       </c>
       <c r="D64">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E64" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>69</v>
       </c>
@@ -2081,13 +2339,17 @@
         <v>90</v>
       </c>
       <c r="D65">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E65" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>71</v>
       </c>
@@ -2098,13 +2360,17 @@
         <v>100</v>
       </c>
       <c r="D66">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="E66" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>72</v>
       </c>
@@ -2115,13 +2381,17 @@
         <v>85</v>
       </c>
       <c r="D67">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E67" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <f t="shared" ref="F67:F130" si="1">ROUND(D67,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -2132,13 +2402,17 @@
         <v>95</v>
       </c>
       <c r="D68">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E68" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -2149,13 +2423,17 @@
         <v>100</v>
       </c>
       <c r="D69">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E69" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>75</v>
       </c>
@@ -2166,13 +2444,17 @@
         <v>100</v>
       </c>
       <c r="D70">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="E70" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>76</v>
       </c>
@@ -2183,13 +2465,17 @@
         <v>100</v>
       </c>
       <c r="D71">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E71" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -2200,13 +2486,17 @@
         <v>90</v>
       </c>
       <c r="D72">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E72" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>78</v>
       </c>
@@ -2217,13 +2507,17 @@
         <v>85</v>
       </c>
       <c r="D73">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E73" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>79</v>
       </c>
@@ -2234,13 +2528,17 @@
         <v>95</v>
       </c>
       <c r="D74">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E74" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>80</v>
       </c>
@@ -2251,13 +2549,17 @@
         <v>100</v>
       </c>
       <c r="D75">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E75" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -2268,13 +2570,17 @@
         <v>100</v>
       </c>
       <c r="D76">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E76" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -2285,13 +2591,17 @@
         <v>100</v>
       </c>
       <c r="D77">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E77" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -2302,13 +2612,17 @@
         <v>100</v>
       </c>
       <c r="D78">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E78" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -2319,13 +2633,17 @@
         <v>100</v>
       </c>
       <c r="D79">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E79" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>86</v>
       </c>
@@ -2336,13 +2654,17 @@
         <v>100</v>
       </c>
       <c r="D80">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E80" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -2353,13 +2675,17 @@
         <v>100</v>
       </c>
       <c r="D81">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E81" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -2370,13 +2696,17 @@
         <v>100</v>
       </c>
       <c r="D82">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E82" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -2387,13 +2717,17 @@
         <v>100</v>
       </c>
       <c r="D83">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E83" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -2404,13 +2738,17 @@
         <v>100</v>
       </c>
       <c r="D84">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E84" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -2421,13 +2759,17 @@
         <v>100</v>
       </c>
       <c r="D85">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E85" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>93</v>
       </c>
@@ -2438,13 +2780,17 @@
         <v>100</v>
       </c>
       <c r="D86">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E86" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>94</v>
       </c>
@@ -2455,13 +2801,17 @@
         <v>100</v>
       </c>
       <c r="D87">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E87" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>95</v>
       </c>
@@ -2472,13 +2822,17 @@
         <v>100</v>
       </c>
       <c r="D88">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E88" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>96</v>
       </c>
@@ -2489,13 +2843,17 @@
         <v>100</v>
       </c>
       <c r="D89">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E89" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>97</v>
       </c>
@@ -2506,13 +2864,17 @@
         <v>100</v>
       </c>
       <c r="D90">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E90" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>98</v>
       </c>
@@ -2523,13 +2885,17 @@
         <v>100</v>
       </c>
       <c r="D91">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E91" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F91">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>99</v>
       </c>
@@ -2540,13 +2906,17 @@
         <v>100</v>
       </c>
       <c r="D92">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E92" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>100</v>
       </c>
@@ -2557,13 +2927,17 @@
         <v>100</v>
       </c>
       <c r="D93">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E93" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F93">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>101</v>
       </c>
@@ -2574,13 +2948,17 @@
         <v>100</v>
       </c>
       <c r="D94">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E94" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F94">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>102</v>
       </c>
@@ -2591,13 +2969,17 @@
         <v>100</v>
       </c>
       <c r="D95">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="E95" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F95">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>104</v>
       </c>
@@ -2608,13 +2990,17 @@
         <v>100</v>
       </c>
       <c r="D96">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E96" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F96">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>105</v>
       </c>
@@ -2625,13 +3011,17 @@
         <v>100</v>
       </c>
       <c r="D97">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E97" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F97">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>106</v>
       </c>
@@ -2642,13 +3032,17 @@
         <v>100</v>
       </c>
       <c r="D98">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E98" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F98">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>107</v>
       </c>
@@ -2659,13 +3053,17 @@
         <v>100</v>
       </c>
       <c r="D99">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E99" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F99">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>108</v>
       </c>
@@ -2676,13 +3074,17 @@
         <v>90</v>
       </c>
       <c r="D100">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E100" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F100">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>109</v>
       </c>
@@ -2693,13 +3095,17 @@
         <v>100</v>
       </c>
       <c r="D101">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E101" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F101">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>110</v>
       </c>
@@ -2710,13 +3116,17 @@
         <v>100</v>
       </c>
       <c r="D102">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E102" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F102">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>111</v>
       </c>
@@ -2727,13 +3137,17 @@
         <v>95</v>
       </c>
       <c r="D103">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="E103" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F103">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>112</v>
       </c>
@@ -2744,13 +3158,17 @@
         <v>100</v>
       </c>
       <c r="D104">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E104" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F104">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>113</v>
       </c>
@@ -2761,13 +3179,17 @@
         <v>100</v>
       </c>
       <c r="D105">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E105" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F105">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>115</v>
       </c>
@@ -2778,13 +3200,17 @@
         <v>100</v>
       </c>
       <c r="D106">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E106" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F106">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>116</v>
       </c>
@@ -2795,13 +3221,17 @@
         <v>95</v>
       </c>
       <c r="D107">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E107" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F107">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>117</v>
       </c>
@@ -2812,13 +3242,17 @@
         <v>100</v>
       </c>
       <c r="D108">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E108" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F108">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>118</v>
       </c>
@@ -2829,13 +3263,17 @@
         <v>100</v>
       </c>
       <c r="D109">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E109" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F109">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>119</v>
       </c>
@@ -2846,13 +3284,17 @@
         <v>90</v>
       </c>
       <c r="D110">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E110" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F110">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>120</v>
       </c>
@@ -2863,13 +3305,17 @@
         <v>90</v>
       </c>
       <c r="D111">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E111" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F111">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>121</v>
       </c>
@@ -2880,13 +3326,17 @@
         <v>85</v>
       </c>
       <c r="D112">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E112" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F112">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>122</v>
       </c>
@@ -2897,13 +3347,17 @@
         <v>100</v>
       </c>
       <c r="D113">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E113" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F113">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>123</v>
       </c>
@@ -2914,13 +3368,17 @@
         <v>30</v>
       </c>
       <c r="D114">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E114" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F114">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>124</v>
       </c>
@@ -2931,13 +3389,17 @@
         <v>100</v>
       </c>
       <c r="D115">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E115" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F115">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>126</v>
       </c>
@@ -2948,13 +3410,17 @@
         <v>70</v>
       </c>
       <c r="D116">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E116" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F116">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>127</v>
       </c>
@@ -2965,13 +3431,17 @@
         <v>90</v>
       </c>
       <c r="D117">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E117" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F117">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>128</v>
       </c>
@@ -2982,13 +3452,17 @@
         <v>100</v>
       </c>
       <c r="D118">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E118" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F118">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>129</v>
       </c>
@@ -2999,13 +3473,17 @@
         <v>100</v>
       </c>
       <c r="D119">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E119" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F119">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>130</v>
       </c>
@@ -3016,13 +3494,17 @@
         <v>95</v>
       </c>
       <c r="D120">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E120" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F120">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>131</v>
       </c>
@@ -3033,13 +3515,17 @@
         <v>100</v>
       </c>
       <c r="D121">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="E121" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F121">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>132</v>
       </c>
@@ -3050,13 +3536,17 @@
         <v>30</v>
       </c>
       <c r="D122">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E122" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F122">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>133</v>
       </c>
@@ -3067,13 +3557,17 @@
         <v>90</v>
       </c>
       <c r="D123">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E123" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F123">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>134</v>
       </c>
@@ -3084,13 +3578,17 @@
         <v>100</v>
       </c>
       <c r="D124">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E124" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F124">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>135</v>
       </c>
@@ -3101,13 +3599,17 @@
         <v>100</v>
       </c>
       <c r="D125">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E125" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F125">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>137</v>
       </c>
@@ -3118,13 +3620,17 @@
         <v>100</v>
       </c>
       <c r="D126">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E126" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F126">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>138</v>
       </c>
@@ -3135,13 +3641,17 @@
         <v>95</v>
       </c>
       <c r="D127">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E127" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F127">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>139</v>
       </c>
@@ -3152,13 +3662,17 @@
         <v>100</v>
       </c>
       <c r="D128">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E128" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F128">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>140</v>
       </c>
@@ -3169,13 +3683,17 @@
         <v>100</v>
       </c>
       <c r="D129">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E129" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F129">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>141</v>
       </c>
@@ -3186,13 +3704,17 @@
         <v>85</v>
       </c>
       <c r="D130">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E130" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F130">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>142</v>
       </c>
@@ -3203,13 +3725,17 @@
         <v>100</v>
       </c>
       <c r="D131">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E131" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F131">
+        <f t="shared" ref="F131:F184" si="2">ROUND(D131,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>143</v>
       </c>
@@ -3220,13 +3746,17 @@
         <v>100</v>
       </c>
       <c r="D132">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E132" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F132">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>144</v>
       </c>
@@ -3237,13 +3767,17 @@
         <v>85</v>
       </c>
       <c r="D133">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E133" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F133">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>145</v>
       </c>
@@ -3254,13 +3788,17 @@
         <v>30</v>
       </c>
       <c r="D134">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E134" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F134">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>146</v>
       </c>
@@ -3271,13 +3809,17 @@
         <v>100</v>
       </c>
       <c r="D135">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E135" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F135">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>148</v>
       </c>
@@ -3288,13 +3830,17 @@
         <v>100</v>
       </c>
       <c r="D136">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E136" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F136">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>149</v>
       </c>
@@ -3305,13 +3851,17 @@
         <v>100</v>
       </c>
       <c r="D137">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E137" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F137">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>150</v>
       </c>
@@ -3322,13 +3872,17 @@
         <v>100</v>
       </c>
       <c r="D138">
-        <v>35</v>
+        <v>17.5</v>
       </c>
       <c r="E138" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F138">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>151</v>
       </c>
@@ -3339,13 +3893,17 @@
         <v>100</v>
       </c>
       <c r="D139">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E139" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F139">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>152</v>
       </c>
@@ -3356,13 +3914,17 @@
         <v>100</v>
       </c>
       <c r="D140">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E140" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F140">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>153</v>
       </c>
@@ -3373,13 +3935,17 @@
         <v>70</v>
       </c>
       <c r="D141">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E141" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F141">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>154</v>
       </c>
@@ -3390,13 +3956,17 @@
         <v>90</v>
       </c>
       <c r="D142">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E142" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F142">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>155</v>
       </c>
@@ -3407,13 +3977,17 @@
         <v>75</v>
       </c>
       <c r="D143">
-        <v>35</v>
+        <v>17.5</v>
       </c>
       <c r="E143" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F143">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>156</v>
       </c>
@@ -3424,13 +3998,17 @@
         <v>100</v>
       </c>
       <c r="D144">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="E144" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F144">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>157</v>
       </c>
@@ -3441,13 +4019,17 @@
         <v>100</v>
       </c>
       <c r="D145">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E145" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F145">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>159</v>
       </c>
@@ -3458,13 +4040,17 @@
         <v>100</v>
       </c>
       <c r="D146">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="E146" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F146">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>160</v>
       </c>
@@ -3475,13 +4061,17 @@
         <v>100</v>
       </c>
       <c r="D147">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E147" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F147">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>161</v>
       </c>
@@ -3492,13 +4082,17 @@
         <v>100</v>
       </c>
       <c r="D148">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E148" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F148">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>162</v>
       </c>
@@ -3509,13 +4103,17 @@
         <v>100</v>
       </c>
       <c r="D149">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E149" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F149">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>163</v>
       </c>
@@ -3526,13 +4124,17 @@
         <v>90</v>
       </c>
       <c r="D150">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E150" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F150">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>164</v>
       </c>
@@ -3543,13 +4145,17 @@
         <v>100</v>
       </c>
       <c r="D151">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E151" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F151">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>165</v>
       </c>
@@ -3560,13 +4166,17 @@
         <v>100</v>
       </c>
       <c r="D152">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E152" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F152">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>166</v>
       </c>
@@ -3577,13 +4187,17 @@
         <v>80</v>
       </c>
       <c r="D153">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E153" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F153">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>167</v>
       </c>
@@ -3594,13 +4208,17 @@
         <v>100</v>
       </c>
       <c r="D154">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="E154" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F154">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>168</v>
       </c>
@@ -3611,13 +4229,17 @@
         <v>100</v>
       </c>
       <c r="D155">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E155" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F155">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>170</v>
       </c>
@@ -3628,13 +4250,17 @@
         <v>90</v>
       </c>
       <c r="D156">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E156" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F156">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>171</v>
       </c>
@@ -3645,13 +4271,17 @@
         <v>90</v>
       </c>
       <c r="D157">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E157" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F157">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>172</v>
       </c>
@@ -3662,13 +4292,17 @@
         <v>90</v>
       </c>
       <c r="D158">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E158" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F158">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>173</v>
       </c>
@@ -3679,13 +4313,17 @@
         <v>90</v>
       </c>
       <c r="D159">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E159" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F159">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>174</v>
       </c>
@@ -3696,13 +4334,17 @@
         <v>100</v>
       </c>
       <c r="D160">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E160" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F160">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>175</v>
       </c>
@@ -3713,13 +4355,17 @@
         <v>100</v>
       </c>
       <c r="D161">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E161" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F161">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>176</v>
       </c>
@@ -3730,13 +4376,17 @@
         <v>95</v>
       </c>
       <c r="D162">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E162" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F162">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>177</v>
       </c>
@@ -3747,13 +4397,17 @@
         <v>100</v>
       </c>
       <c r="D163">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E163" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F163">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>178</v>
       </c>
@@ -3764,13 +4418,17 @@
         <v>80</v>
       </c>
       <c r="D164">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E164" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F164">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>179</v>
       </c>
@@ -3781,13 +4439,17 @@
         <v>100</v>
       </c>
       <c r="D165">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E165" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F165">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>181</v>
       </c>
@@ -3798,13 +4460,17 @@
         <v>75</v>
       </c>
       <c r="D166">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E166" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F166">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>182</v>
       </c>
@@ -3815,13 +4481,17 @@
         <v>95</v>
       </c>
       <c r="D167">
-        <v>35</v>
+        <v>17.5</v>
       </c>
       <c r="E167" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F167">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>183</v>
       </c>
@@ -3832,13 +4502,17 @@
         <v>90</v>
       </c>
       <c r="D168">
-        <v>25</v>
+        <v>12.5</v>
       </c>
       <c r="E168" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F168">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>184</v>
       </c>
@@ -3849,13 +4523,17 @@
         <v>100</v>
       </c>
       <c r="D169">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E169" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F169">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>185</v>
       </c>
@@ -3866,13 +4544,17 @@
         <v>100</v>
       </c>
       <c r="D170">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E170" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F170">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>186</v>
       </c>
@@ -3883,13 +4565,17 @@
         <v>90</v>
       </c>
       <c r="D171">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E171" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F171">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>187</v>
       </c>
@@ -3900,13 +4586,17 @@
         <v>100</v>
       </c>
       <c r="D172">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E172" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F172">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>188</v>
       </c>
@@ -3917,13 +4607,17 @@
         <v>100</v>
       </c>
       <c r="D173">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E173" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F173">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>189</v>
       </c>
@@ -3934,13 +4628,17 @@
         <v>100</v>
       </c>
       <c r="D174">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E174" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F174">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>190</v>
       </c>
@@ -3951,13 +4649,17 @@
         <v>100</v>
       </c>
       <c r="D175">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E175" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F175">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>192</v>
       </c>
@@ -3968,13 +4670,17 @@
         <v>100</v>
       </c>
       <c r="D176">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E176" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F176">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>193</v>
       </c>
@@ -3985,13 +4691,17 @@
         <v>90</v>
       </c>
       <c r="D177">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E177" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F177">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>194</v>
       </c>
@@ -4002,13 +4712,17 @@
         <v>80</v>
       </c>
       <c r="D178">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E178" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F178">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>195</v>
       </c>
@@ -4019,13 +4733,17 @@
         <v>85</v>
       </c>
       <c r="D179">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E179" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F179">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>196</v>
       </c>
@@ -4036,13 +4754,17 @@
         <v>100</v>
       </c>
       <c r="D180">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E180" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F180">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>197</v>
       </c>
@@ -4053,13 +4775,17 @@
         <v>100</v>
       </c>
       <c r="D181">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="E181" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F181">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>198</v>
       </c>
@@ -4070,13 +4796,17 @@
         <v>100</v>
       </c>
       <c r="D182">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E182" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F182">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>199</v>
       </c>
@@ -4087,13 +4817,17 @@
         <v>100</v>
       </c>
       <c r="D183">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E183" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F183">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>200</v>
       </c>
@@ -4104,13 +4838,18 @@
         <v>95</v>
       </c>
       <c r="D184">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="E184" t="s">
         <v>191</v>
       </c>
+      <c r="F184">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
started working on move side effects
</commit_message>
<xml_diff>
--- a/moves.xlsx
+++ b/moves.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="210">
   <si>
     <t>Bug Bite</t>
   </si>
@@ -635,6 +635,15 @@
   </si>
   <si>
     <t>pp1</t>
+  </si>
+  <si>
+    <t>health</t>
+  </si>
+  <si>
+    <t>stats</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
@@ -970,10 +979,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F184"/>
+  <dimension ref="A1:I184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,7 +995,7 @@
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>201</v>
       </c>
@@ -1004,8 +1014,17 @@
       <c r="F1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H1" t="s">
+        <v>208</v>
+      </c>
+      <c r="I1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1025,8 +1044,17 @@
         <f>ROUND(D2,0)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1046,8 +1074,17 @@
         <f t="shared" ref="F3:F66" si="0">ROUND(D3,0)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>-2</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1067,8 +1104,17 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1088,8 +1134,17 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>0.5</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1109,8 +1164,17 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1130,8 +1194,17 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1151,8 +1224,17 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1172,8 +1254,17 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1193,8 +1284,17 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>-3.5</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1214,8 +1314,17 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>-1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1235,8 +1344,17 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1256,8 +1374,17 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1277,8 +1404,17 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1299,7 +1435,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
added 3/5 in-battle stats change
</commit_message>
<xml_diff>
--- a/moves.xlsx
+++ b/moves.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="212">
   <si>
     <t>Bug Bite</t>
   </si>
@@ -280,15 +280,9 @@
     <t>Wing Attack</t>
   </si>
   <si>
-    <t>Roost</t>
-  </si>
-  <si>
     <t>Feather Dance</t>
   </si>
   <si>
-    <t>Tailwind</t>
-  </si>
-  <si>
     <t>Astonish</t>
   </si>
   <si>
@@ -644,6 +638,18 @@
   </si>
   <si>
     <t>status</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>Air Slash</t>
+  </si>
+  <si>
+    <t>Brave Bird</t>
   </si>
 </sst>
 </file>
@@ -982,8 +988,8 @@
   <dimension ref="A1:I184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H184" sqref="H184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,31 +1003,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" t="s">
         <v>201</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F1" t="s">
         <v>202</v>
       </c>
-      <c r="C1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" t="s">
         <v>206</v>
       </c>
-      <c r="E1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>207</v>
-      </c>
-      <c r="H1" t="s">
-        <v>208</v>
-      </c>
-      <c r="I1" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1044,13 +1050,7 @@
         <f>ROUND(D2,0)</f>
         <v>10</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
       <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
         <v>0</v>
       </c>
     </row>
@@ -1074,14 +1074,8 @@
         <f t="shared" ref="F3:F66" si="0">ROUND(D3,0)</f>
         <v>5</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
       <c r="H3">
-        <v>-2</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
+        <v>-2.5</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1104,13 +1098,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
       <c r="H4">
-        <v>4</v>
-      </c>
-      <c r="I4">
         <v>0</v>
       </c>
     </row>
@@ -1134,13 +1122,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G5">
-        <v>0.5</v>
-      </c>
       <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
         <v>0</v>
       </c>
     </row>
@@ -1164,13 +1146,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
       <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
         <v>0</v>
       </c>
     </row>
@@ -1194,13 +1170,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
       <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
         <v>0</v>
       </c>
     </row>
@@ -1224,14 +1194,8 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
       <c r="H8">
         <v>0</v>
-      </c>
-      <c r="I8">
-        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1254,14 +1218,8 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
       <c r="H9">
-        <v>10</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1284,14 +1242,8 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
       <c r="H10">
-        <v>-3.5</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
+        <v>-3.75</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1314,14 +1266,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
       <c r="H11">
-        <v>-1</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
+        <v>-1.5</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1344,14 +1290,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
       <c r="H12">
         <v>0</v>
-      </c>
-      <c r="I12">
-        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1374,13 +1314,7 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
       <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
         <v>0</v>
       </c>
     </row>
@@ -1404,13 +1338,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
       <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
         <v>0</v>
       </c>
     </row>
@@ -1434,6 +1362,9 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1455,8 +1386,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1476,8 +1410,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>-2.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1497,8 +1434,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1518,8 +1458,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1539,8 +1482,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>-1.75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1560,8 +1506,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1581,8 +1530,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1602,8 +1554,11 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1623,8 +1578,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1644,8 +1602,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1665,8 +1626,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1686,8 +1650,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1707,8 +1674,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1728,8 +1698,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1749,8 +1722,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1770,8 +1746,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1791,8 +1770,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1812,8 +1794,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1833,8 +1818,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1854,8 +1842,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1875,8 +1866,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1896,8 +1890,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -1917,8 +1914,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -1938,8 +1938,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -1959,8 +1962,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -1980,8 +1986,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -2001,8 +2010,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -2022,8 +2034,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -2043,8 +2058,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -2064,8 +2082,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H45">
+        <v>-1.75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -2085,8 +2106,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -2106,8 +2130,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -2127,8 +2154,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -2148,8 +2178,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -2169,8 +2202,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -2190,8 +2226,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H51">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -2211,8 +2250,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -2232,8 +2274,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H53">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -2253,8 +2298,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -2274,8 +2322,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -2295,8 +2346,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H56">
+        <v>-2.75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -2316,8 +2370,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H57" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>62</v>
       </c>
@@ -2337,8 +2394,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -2358,8 +2418,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -2379,8 +2442,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -2400,8 +2466,11 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>66</v>
       </c>
@@ -2421,8 +2490,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H62">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -2442,8 +2514,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -2463,8 +2538,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>69</v>
       </c>
@@ -2484,8 +2562,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>71</v>
       </c>
@@ -2505,8 +2586,11 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>72</v>
       </c>
@@ -2526,8 +2610,11 @@
         <f t="shared" ref="F67:F130" si="1">ROUND(D67,0)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -2547,8 +2634,11 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -2568,8 +2658,11 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>75</v>
       </c>
@@ -2589,8 +2682,11 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>76</v>
       </c>
@@ -2610,8 +2706,11 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -2631,8 +2730,11 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H72">
+        <v>-1.25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>78</v>
       </c>
@@ -2652,8 +2754,11 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>79</v>
       </c>
@@ -2673,8 +2778,11 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>80</v>
       </c>
@@ -2694,8 +2802,11 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>82</v>
       </c>
@@ -2715,8 +2826,11 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>83</v>
       </c>
@@ -2736,8 +2850,11 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -2757,8 +2874,11 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>85</v>
       </c>
@@ -2778,8 +2898,11 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>86</v>
       </c>
@@ -2799,8 +2922,11 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>87</v>
       </c>
@@ -2820,16 +2946,19 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>88</v>
+        <v>210</v>
       </c>
       <c r="B82">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C82">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D82">
         <v>10</v>
@@ -2841,10 +2970,13 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B83">
         <v>60</v>
@@ -2862,31 +2994,37 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H83">
+        <v>-1.75</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>90</v>
+        <v>211</v>
       </c>
       <c r="B84">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="C84">
         <v>100</v>
       </c>
       <c r="D84">
-        <v>10</v>
+        <v>7.5</v>
       </c>
       <c r="E84" t="s">
         <v>81</v>
       </c>
       <c r="F84">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B85">
         <v>30</v>
@@ -2898,16 +3036,19 @@
         <v>7.5</v>
       </c>
       <c r="E85" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F85">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B86">
         <v>65</v>
@@ -2919,16 +3060,19 @@
         <v>5</v>
       </c>
       <c r="E86" t="s">
+        <v>90</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>92</v>
-      </c>
-      <c r="F86">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>94</v>
       </c>
       <c r="B87">
         <v>30</v>
@@ -2940,16 +3084,19 @@
         <v>15</v>
       </c>
       <c r="E87" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F87">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B88">
         <v>80</v>
@@ -2961,16 +3108,19 @@
         <v>7.5</v>
       </c>
       <c r="E88" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F88">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H88">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B89">
         <v>85</v>
@@ -2982,16 +3132,19 @@
         <v>5</v>
       </c>
       <c r="E89" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F89">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H89">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B90">
         <v>70</v>
@@ -3003,16 +3156,19 @@
         <v>2.5</v>
       </c>
       <c r="E90" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F90">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B91">
         <v>60</v>
@@ -3024,16 +3180,19 @@
         <v>10</v>
       </c>
       <c r="E91" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F91">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B92">
         <v>80</v>
@@ -3045,16 +3204,19 @@
         <v>5</v>
       </c>
       <c r="E92" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F92">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B93">
         <v>100</v>
@@ -3066,16 +3228,19 @@
         <v>2.5</v>
       </c>
       <c r="E93" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F93">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -3087,16 +3252,19 @@
         <v>2.5</v>
       </c>
       <c r="E94" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F94">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B95">
         <v>20</v>
@@ -3108,16 +3276,19 @@
         <v>12.5</v>
       </c>
       <c r="E95" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F95">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B96">
         <v>25</v>
@@ -3129,16 +3300,19 @@
         <v>15</v>
       </c>
       <c r="E96" t="s">
+        <v>101</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>103</v>
-      </c>
-      <c r="F96">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>105</v>
       </c>
       <c r="B97">
         <v>75</v>
@@ -3150,16 +3324,19 @@
         <v>5</v>
       </c>
       <c r="E97" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F97">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -3171,16 +3348,19 @@
         <v>10</v>
       </c>
       <c r="E98" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F98">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B99">
         <v>90</v>
@@ -3192,16 +3372,19 @@
         <v>7.5</v>
       </c>
       <c r="E99" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F99">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -3213,16 +3396,19 @@
         <v>5</v>
       </c>
       <c r="E100" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F100">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B101">
         <v>60</v>
@@ -3234,16 +3420,19 @@
         <v>10</v>
       </c>
       <c r="E101" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F101">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B102">
         <v>40</v>
@@ -3255,16 +3444,19 @@
         <v>7.5</v>
       </c>
       <c r="E102" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F102">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B103">
         <v>55</v>
@@ -3276,16 +3468,19 @@
         <v>12.5</v>
       </c>
       <c r="E103" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F103">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -3297,37 +3492,43 @@
         <v>2.5</v>
       </c>
       <c r="E104" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F104">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>111</v>
+      </c>
+      <c r="B105">
+        <v>100</v>
+      </c>
+      <c r="C105">
+        <v>100</v>
+      </c>
+      <c r="D105">
+        <v>5</v>
+      </c>
+      <c r="E105" t="s">
+        <v>112</v>
+      </c>
+      <c r="F105">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>113</v>
-      </c>
-      <c r="B105">
-        <v>100</v>
-      </c>
-      <c r="C105">
-        <v>100</v>
-      </c>
-      <c r="D105">
-        <v>5</v>
-      </c>
-      <c r="E105" t="s">
-        <v>114</v>
-      </c>
-      <c r="F105">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>115</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -3339,16 +3540,19 @@
         <v>15</v>
       </c>
       <c r="E106" t="s">
+        <v>112</v>
+      </c>
+      <c r="F106">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="H106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>114</v>
-      </c>
-      <c r="F106">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>116</v>
       </c>
       <c r="B107">
         <v>55</v>
@@ -3360,16 +3564,19 @@
         <v>7.5</v>
       </c>
       <c r="E107" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F107">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H107">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B108">
         <v>20</v>
@@ -3381,16 +3588,19 @@
         <v>5</v>
       </c>
       <c r="E108" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F108">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H108">
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -3402,16 +3612,19 @@
         <v>7.5</v>
       </c>
       <c r="E109" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F109">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H109">
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B110">
         <v>50</v>
@@ -3423,16 +3636,19 @@
         <v>5</v>
       </c>
       <c r="E110" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F110">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B111">
         <v>25</v>
@@ -3444,16 +3660,19 @@
         <v>5</v>
       </c>
       <c r="E111" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F111">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B112">
         <v>65</v>
@@ -3465,16 +3684,19 @@
         <v>10</v>
       </c>
       <c r="E112" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F112">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B113">
         <v>90</v>
@@ -3486,16 +3708,19 @@
         <v>5</v>
       </c>
       <c r="E113" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F113">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H113">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B114">
         <v>10000</v>
@@ -3507,16 +3732,19 @@
         <v>2.5</v>
       </c>
       <c r="E114" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F114">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B115">
         <v>65</v>
@@ -3528,16 +3756,19 @@
         <v>10</v>
       </c>
       <c r="E115" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F115">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H115">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B116">
         <v>110</v>
@@ -3549,16 +3780,19 @@
         <v>2.5</v>
       </c>
       <c r="E116" t="s">
+        <v>123</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>125</v>
-      </c>
-      <c r="F116">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>127</v>
       </c>
       <c r="B117">
         <v>30</v>
@@ -3570,16 +3804,19 @@
         <v>10</v>
       </c>
       <c r="E117" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F117">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B118">
         <v>90</v>
@@ -3591,16 +3828,19 @@
         <v>5</v>
       </c>
       <c r="E118" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F118">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B119">
         <v>75</v>
@@ -3612,16 +3852,19 @@
         <v>7.5</v>
       </c>
       <c r="E119" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F119">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B120">
         <v>55</v>
@@ -3633,16 +3876,19 @@
         <v>7.5</v>
       </c>
       <c r="E120" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F120">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H120">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B121">
         <v>40</v>
@@ -3654,16 +3900,19 @@
         <v>12.5</v>
       </c>
       <c r="E121" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F121">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B122">
         <v>10000</v>
@@ -3675,16 +3924,19 @@
         <v>2.5</v>
       </c>
       <c r="E122" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F122">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B123">
         <v>100</v>
@@ -3696,16 +3948,19 @@
         <v>5</v>
       </c>
       <c r="E123" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F123">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H123">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B124">
         <v>60</v>
@@ -3717,37 +3972,43 @@
         <v>5</v>
       </c>
       <c r="E124" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F124">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>133</v>
+      </c>
+      <c r="B125">
+        <v>0</v>
+      </c>
+      <c r="C125">
+        <v>100</v>
+      </c>
+      <c r="D125">
+        <v>5</v>
+      </c>
+      <c r="E125" t="s">
+        <v>134</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H125">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>135</v>
-      </c>
-      <c r="B125">
-        <v>0</v>
-      </c>
-      <c r="C125">
-        <v>100</v>
-      </c>
-      <c r="D125">
-        <v>5</v>
-      </c>
-      <c r="E125" t="s">
-        <v>136</v>
-      </c>
-      <c r="F125">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>137</v>
       </c>
       <c r="B126">
         <v>85</v>
@@ -3759,16 +4020,19 @@
         <v>7.5</v>
       </c>
       <c r="E126" t="s">
+        <v>134</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>136</v>
-      </c>
-      <c r="F126">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>138</v>
       </c>
       <c r="B127">
         <v>50</v>
@@ -3780,16 +4044,19 @@
         <v>15</v>
       </c>
       <c r="E127" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F127">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -3801,16 +4068,19 @@
         <v>20</v>
       </c>
       <c r="E128" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F128">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B129">
         <v>70</v>
@@ -3822,16 +4092,19 @@
         <v>5</v>
       </c>
       <c r="E129" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F129">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B130">
         <v>15</v>
@@ -3843,16 +4116,19 @@
         <v>5</v>
       </c>
       <c r="E130" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F130">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B131">
         <v>120</v>
@@ -3864,16 +4140,19 @@
         <v>7.5</v>
       </c>
       <c r="E131" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F131">
         <f t="shared" ref="F131:F184" si="2">ROUND(D131,0)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -3885,16 +4164,19 @@
         <v>7.5</v>
       </c>
       <c r="E132" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F132">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B133">
         <v>15</v>
@@ -3906,16 +4188,19 @@
         <v>10</v>
       </c>
       <c r="E133" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F133">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B134">
         <v>10000</v>
@@ -3927,16 +4212,19 @@
         <v>2.5</v>
       </c>
       <c r="E134" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F134">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B135">
         <v>40</v>
@@ -3948,16 +4236,19 @@
         <v>15</v>
       </c>
       <c r="E135" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F135">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H135">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -3969,16 +4260,19 @@
         <v>10</v>
       </c>
       <c r="E136" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F136">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H136">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B137">
         <v>50</v>
@@ -3990,16 +4284,19 @@
         <v>7.5</v>
       </c>
       <c r="E137" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F137">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B138">
         <v>15</v>
@@ -4011,16 +4308,19 @@
         <v>17.5</v>
       </c>
       <c r="E138" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F138">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B139">
         <v>65</v>
@@ -4032,16 +4332,19 @@
         <v>10</v>
       </c>
       <c r="E139" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F139">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B140">
         <v>90</v>
@@ -4053,16 +4356,19 @@
         <v>5</v>
       </c>
       <c r="E140" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F140">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B141">
         <v>30</v>
@@ -4074,16 +4380,19 @@
         <v>10</v>
       </c>
       <c r="E141" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F141">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -4095,16 +4404,19 @@
         <v>5</v>
       </c>
       <c r="E142" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F142">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -4116,16 +4428,19 @@
         <v>17.5</v>
       </c>
       <c r="E143" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F143">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B144">
         <v>50</v>
@@ -4137,16 +4452,19 @@
         <v>12.5</v>
       </c>
       <c r="E144" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F144">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B145">
         <v>0</v>
@@ -4158,16 +4476,19 @@
         <v>15</v>
       </c>
       <c r="E145" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F145">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H145">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B146">
         <v>50</v>
@@ -4179,19 +4500,22 @@
         <v>12.5</v>
       </c>
       <c r="E146" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F146">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B147">
-        <v>0</v>
+        <v>-60</v>
       </c>
       <c r="C147">
         <v>100</v>
@@ -4200,16 +4524,19 @@
         <v>5</v>
       </c>
       <c r="E147" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F147">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B148">
         <v>65</v>
@@ -4221,16 +4548,19 @@
         <v>10</v>
       </c>
       <c r="E148" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F148">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B149">
         <v>90</v>
@@ -4242,16 +4572,19 @@
         <v>5</v>
       </c>
       <c r="E149" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F149">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H149">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B150">
         <v>140</v>
@@ -4263,16 +4596,19 @@
         <v>2.5</v>
       </c>
       <c r="E150" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F150">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H150">
+        <v>-1.25</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B151">
         <v>80</v>
@@ -4284,16 +4620,19 @@
         <v>10</v>
       </c>
       <c r="E151" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F151">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -4305,16 +4644,19 @@
         <v>20</v>
       </c>
       <c r="E152" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F152">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -4326,16 +4668,19 @@
         <v>7.5</v>
       </c>
       <c r="E153" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F153">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H153">
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B154">
         <v>60</v>
@@ -4347,16 +4692,19 @@
         <v>12.5</v>
       </c>
       <c r="E154" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F154">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B155">
         <v>60</v>
@@ -4368,16 +4716,19 @@
         <v>2.5</v>
       </c>
       <c r="E155" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F155">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H155">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B156">
         <v>25</v>
@@ -4389,16 +4740,19 @@
         <v>5</v>
       </c>
       <c r="E156" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F156">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B157">
         <v>75</v>
@@ -4410,16 +4764,19 @@
         <v>5</v>
       </c>
       <c r="E157" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F157">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B158">
         <v>30</v>
@@ -4431,16 +4788,19 @@
         <v>10</v>
       </c>
       <c r="E158" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F158">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B159">
         <v>50</v>
@@ -4452,16 +4812,19 @@
         <v>7.5</v>
       </c>
       <c r="E159" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F159">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -4473,16 +4836,19 @@
         <v>10</v>
       </c>
       <c r="E160" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F160">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H160">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B161">
         <v>40</v>
@@ -4494,16 +4860,19 @@
         <v>10</v>
       </c>
       <c r="E161" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F161">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B162">
         <v>60</v>
@@ -4515,16 +4884,19 @@
         <v>7.5</v>
       </c>
       <c r="E162" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F162">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H162">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B163">
         <v>50</v>
@@ -4536,16 +4908,19 @@
         <v>7.5</v>
       </c>
       <c r="E163" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F163">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B164">
         <v>150</v>
@@ -4557,16 +4932,19 @@
         <v>2.5</v>
       </c>
       <c r="E164" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F164">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B165">
         <v>0</v>
@@ -4578,16 +4956,19 @@
         <v>7.5</v>
       </c>
       <c r="E165" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F165">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H165">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B166">
         <v>100</v>
@@ -4599,16 +4980,19 @@
         <v>7.5</v>
       </c>
       <c r="E166" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F166">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H166">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B167">
         <v>50</v>
@@ -4620,16 +5004,19 @@
         <v>17.5</v>
       </c>
       <c r="E167" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F167">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B168">
         <v>70</v>
@@ -4641,16 +5028,19 @@
         <v>12.5</v>
       </c>
       <c r="E168" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F168">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H168">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B169">
         <v>40</v>
@@ -4662,16 +5052,19 @@
         <v>15</v>
       </c>
       <c r="E169" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F169">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B170">
         <v>60</v>
@@ -4683,16 +5076,19 @@
         <v>10</v>
       </c>
       <c r="E170" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F170">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B171">
         <v>90</v>
@@ -4704,16 +5100,19 @@
         <v>5</v>
       </c>
       <c r="E171" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F171">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B172">
         <v>70</v>
@@ -4725,16 +5124,19 @@
         <v>5</v>
       </c>
       <c r="E172" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F172">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B173">
         <v>80</v>
@@ -4746,16 +5148,19 @@
         <v>10</v>
       </c>
       <c r="E173" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F173">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B174">
         <v>0</v>
@@ -4767,16 +5172,19 @@
         <v>7.5</v>
       </c>
       <c r="E174" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F174">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H174">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B175">
         <v>40</v>
@@ -4788,16 +5196,19 @@
         <v>15</v>
       </c>
       <c r="E175" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F175">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H175">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B176">
         <v>65</v>
@@ -4809,16 +5220,19 @@
         <v>10</v>
       </c>
       <c r="E176" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F176">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H176">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B177">
         <v>100</v>
@@ -4830,16 +5244,19 @@
         <v>5</v>
       </c>
       <c r="E177" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F177">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B178">
         <v>110</v>
@@ -4851,16 +5268,19 @@
         <v>2.5</v>
       </c>
       <c r="E178" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F178">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B179">
         <v>90</v>
@@ -4872,16 +5292,19 @@
         <v>5</v>
       </c>
       <c r="E179" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F179">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H179">
+        <v>-5.5</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B180">
         <v>90</v>
@@ -4893,16 +5316,19 @@
         <v>7.5</v>
       </c>
       <c r="E180" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F180">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B181">
         <v>80</v>
@@ -4914,16 +5340,19 @@
         <v>7.5</v>
       </c>
       <c r="E181" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F181">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B182">
         <v>60</v>
@@ -4935,16 +5364,19 @@
         <v>10</v>
       </c>
       <c r="E182" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F182">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B183">
         <v>0</v>
@@ -4956,16 +5388,19 @@
         <v>20</v>
       </c>
       <c r="E183" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F183">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H183">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B184">
         <v>110</v>
@@ -4977,11 +5412,14 @@
         <v>2.5</v>
       </c>
       <c r="E184" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F184">
         <f t="shared" si="2"/>
         <v>3</v>
+      </c>
+      <c r="H184">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added recoil and regain effects for moves
</commit_message>
<xml_diff>
--- a/moves.xlsx
+++ b/moves.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GHO1KOR\Downloads\PokemonBattle-master\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="213">
   <si>
     <t>Bug Bite</t>
   </si>
@@ -655,12 +650,15 @@
   </si>
   <si>
     <t>Brave Bird</t>
+  </si>
+  <si>
+    <t>3,-1.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -996,8 +994,8 @@
   <dimension ref="A1:I184"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A157" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I185" sqref="I185"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2435,8 +2433,8 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H53">
-        <v>-1.5</v>
+      <c r="H53" t="s">
+        <v>212</v>
       </c>
       <c r="I53">
         <v>0</v>

</xml_diff>

<commit_message>
restructured battle scene; multiple hits added
</commit_message>
<xml_diff>
--- a/moves.xlsx
+++ b/moves.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sheet1!$A$1:$I$184</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="214">
   <si>
     <t>Bug Bite</t>
   </si>
@@ -653,6 +656,9 @@
   </si>
   <si>
     <t>3,-1.5</t>
+  </si>
+  <si>
+    <t>8;5000</t>
   </si>
 </sst>
 </file>
@@ -687,8 +693,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -991,11 +998,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I184"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G185" sqref="G185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,6 +1064,9 @@
         <f>ROUND(D2,0)</f>
         <v>10</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H2">
         <v>0</v>
       </c>
@@ -1083,6 +1094,9 @@
         <f t="shared" ref="F3:F66" si="0">ROUND(D3,0)</f>
         <v>5</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H3">
         <v>-2.5</v>
       </c>
@@ -1110,6 +1124,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H4">
         <v>0</v>
       </c>
@@ -1137,6 +1154,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="G5" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H5">
         <v>0</v>
       </c>
@@ -1163,6 +1183,9 @@
       <c r="F6">
         <f t="shared" si="0"/>
         <v>5</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1191,6 +1214,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="G7" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H7">
         <v>0</v>
       </c>
@@ -1218,6 +1244,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="G8" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H8">
         <v>0</v>
       </c>
@@ -1245,6 +1274,9 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
+      <c r="G9" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H9">
         <v>4</v>
       </c>
@@ -1252,7 +1284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1272,6 +1304,9 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
+      <c r="G10">
+        <v>1000</v>
+      </c>
       <c r="H10">
         <v>-3.75</v>
       </c>
@@ -1298,6 +1333,9 @@
       <c r="F11">
         <f t="shared" si="0"/>
         <v>10</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="H11">
         <v>-1.5</v>
@@ -1326,6 +1364,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="G12" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H12">
         <v>0</v>
       </c>
@@ -1353,6 +1394,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="G13" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H13">
         <v>0</v>
       </c>
@@ -1380,6 +1424,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H14">
         <v>0</v>
       </c>
@@ -1407,6 +1454,9 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
+      <c r="G15" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H15">
         <v>0</v>
       </c>
@@ -1434,6 +1484,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="G16" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H16">
         <v>-2.5</v>
       </c>
@@ -1441,7 +1494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1460,6 +1513,9 @@
       <c r="F17">
         <f t="shared" si="0"/>
         <v>10</v>
+      </c>
+      <c r="G17">
+        <v>1000</v>
       </c>
       <c r="H17">
         <v>-2.75</v>
@@ -1488,6 +1544,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="G18" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H18">
         <v>0</v>
       </c>
@@ -1515,6 +1574,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="G19" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H19">
         <v>0</v>
       </c>
@@ -1522,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1541,6 +1603,9 @@
       <c r="F20">
         <f t="shared" si="0"/>
         <v>5</v>
+      </c>
+      <c r="G20">
+        <v>1000</v>
       </c>
       <c r="H20">
         <v>-1.75</v>
@@ -1569,6 +1634,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="G21" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H21">
         <v>0</v>
       </c>
@@ -1596,6 +1664,9 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
+      <c r="G22" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H22">
         <v>0</v>
       </c>
@@ -1623,6 +1694,9 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
+      <c r="G23" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H23">
         <v>0</v>
       </c>
@@ -1650,6 +1724,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="G24" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H24">
         <v>0</v>
       </c>
@@ -1677,6 +1754,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="G25" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H25">
         <v>0</v>
       </c>
@@ -1704,6 +1784,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="G26" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H26">
         <v>0</v>
       </c>
@@ -1711,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1730,6 +1813,9 @@
       <c r="F27">
         <f t="shared" si="0"/>
         <v>10</v>
+      </c>
+      <c r="G27">
+        <v>1000</v>
       </c>
       <c r="H27" t="s">
         <v>208</v>
@@ -1758,6 +1844,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="G28" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H28">
         <v>0</v>
       </c>
@@ -1785,6 +1874,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="G29" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H29">
         <v>0</v>
       </c>
@@ -1792,7 +1884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1811,6 +1903,9 @@
       <c r="F30">
         <f t="shared" si="0"/>
         <v>5</v>
+      </c>
+      <c r="G30">
+        <v>1000</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -1839,6 +1934,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="G31" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H31">
         <v>0</v>
       </c>
@@ -1866,6 +1964,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="G32" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H32">
         <v>0</v>
       </c>
@@ -1893,6 +1994,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="G33" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H33">
         <v>0</v>
       </c>
@@ -1920,6 +2024,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="G34" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H34">
         <v>0</v>
       </c>
@@ -1947,6 +2054,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="G35" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H35">
         <v>0</v>
       </c>
@@ -1974,6 +2084,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="G36" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H36">
         <v>0</v>
       </c>
@@ -2001,6 +2114,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="G37" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H37">
         <v>0</v>
       </c>
@@ -2028,6 +2144,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="G38" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H38">
         <v>0</v>
       </c>
@@ -2055,6 +2174,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="G39" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H39">
         <v>0</v>
       </c>
@@ -2082,6 +2204,9 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
+      <c r="G40" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H40">
         <v>0</v>
       </c>
@@ -2089,7 +2214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -2108,6 +2233,9 @@
       <c r="F41">
         <f t="shared" si="0"/>
         <v>10</v>
+      </c>
+      <c r="G41">
+        <v>1000</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -2136,6 +2264,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="G42" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H42">
         <v>0</v>
       </c>
@@ -2163,6 +2294,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="G43" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H43">
         <v>0</v>
       </c>
@@ -2190,6 +2324,9 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
+      <c r="G44" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H44">
         <v>0</v>
       </c>
@@ -2197,7 +2334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -2217,6 +2354,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="G45">
+        <v>1000</v>
+      </c>
       <c r="H45">
         <v>-1.75</v>
       </c>
@@ -2224,7 +2364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -2244,6 +2384,9 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
+      <c r="G46">
+        <v>1000</v>
+      </c>
       <c r="H46">
         <v>0</v>
       </c>
@@ -2251,7 +2394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -2270,6 +2413,9 @@
       <c r="F47">
         <f t="shared" si="0"/>
         <v>5</v>
+      </c>
+      <c r="G47">
+        <v>1000</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -2298,6 +2444,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="G48" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H48">
         <v>0</v>
       </c>
@@ -2325,6 +2474,9 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
+      <c r="G49" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H49">
         <v>0</v>
       </c>
@@ -2352,6 +2504,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="G50" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H50">
         <v>-1.5</v>
       </c>
@@ -2379,6 +2534,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="G51" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H51">
         <v>-1.5</v>
       </c>
@@ -2406,6 +2564,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="G52" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H52">
         <v>0</v>
       </c>
@@ -2413,7 +2574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -2433,6 +2594,9 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
+      <c r="G53">
+        <v>1000</v>
+      </c>
       <c r="H53" t="s">
         <v>212</v>
       </c>
@@ -2460,6 +2624,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="G54" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H54">
         <v>0</v>
       </c>
@@ -2487,6 +2654,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="G55" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H55">
         <v>0</v>
       </c>
@@ -2514,6 +2684,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="G56" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H56">
         <v>-2.75</v>
       </c>
@@ -2521,7 +2694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -2540,6 +2713,9 @@
       <c r="F57">
         <f t="shared" si="0"/>
         <v>10</v>
+      </c>
+      <c r="G57">
+        <v>1000</v>
       </c>
       <c r="H57" t="s">
         <v>209</v>
@@ -2568,6 +2744,9 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
+      <c r="G58" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H58">
         <v>0</v>
       </c>
@@ -2595,6 +2774,9 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
+      <c r="G59" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H59">
         <v>0</v>
       </c>
@@ -2622,6 +2804,9 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
+      <c r="G60" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H60">
         <v>0</v>
       </c>
@@ -2649,6 +2834,9 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
+      <c r="G61" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H61">
         <v>0</v>
       </c>
@@ -2676,6 +2864,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="G62" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H62">
         <v>-2.5</v>
       </c>
@@ -2703,6 +2894,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
+      <c r="G63" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H63">
         <v>0</v>
       </c>
@@ -2730,6 +2924,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="G64" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H64">
         <v>0</v>
       </c>
@@ -2757,6 +2954,9 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
+      <c r="G65" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H65">
         <v>0</v>
       </c>
@@ -2784,6 +2984,9 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
+      <c r="G66" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H66">
         <v>0</v>
       </c>
@@ -2811,6 +3014,9 @@
         <f t="shared" ref="F67:F130" si="1">ROUND(D67,0)</f>
         <v>3</v>
       </c>
+      <c r="G67" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H67">
         <v>0</v>
       </c>
@@ -2838,6 +3044,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="G68" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H68">
         <v>0</v>
       </c>
@@ -2865,6 +3074,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="G69" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H69">
         <v>0</v>
       </c>
@@ -2892,6 +3104,9 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
+      <c r="G70" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H70">
         <v>0</v>
       </c>
@@ -2919,6 +3134,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="G71" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H71">
         <v>0</v>
       </c>
@@ -2946,6 +3164,9 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="G72" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H72">
         <v>-1.25</v>
       </c>
@@ -2953,7 +3174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>78</v>
       </c>
@@ -2973,6 +3194,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="G73">
+        <v>1000</v>
+      </c>
       <c r="H73">
         <v>0</v>
       </c>
@@ -3000,6 +3224,9 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="G74" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H74">
         <v>0</v>
       </c>
@@ -3027,6 +3254,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="G75" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H75">
         <v>0</v>
       </c>
@@ -3054,6 +3284,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="G76" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H76">
         <v>0</v>
       </c>
@@ -3081,6 +3314,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="G77" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H77">
         <v>0</v>
       </c>
@@ -3108,6 +3344,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="G78" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H78">
         <v>0</v>
       </c>
@@ -3135,6 +3374,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="G79" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H79">
         <v>0</v>
       </c>
@@ -3162,6 +3404,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="G80" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H80">
         <v>0</v>
       </c>
@@ -3189,6 +3434,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="G81" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H81">
         <v>0</v>
       </c>
@@ -3216,6 +3464,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="G82" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H82">
         <v>0</v>
       </c>
@@ -3243,6 +3494,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="G83" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H83">
         <v>-1.75</v>
       </c>
@@ -3270,6 +3524,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="G84" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H84">
         <v>0</v>
       </c>
@@ -3297,6 +3554,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="G85" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H85">
         <v>0</v>
       </c>
@@ -3324,6 +3584,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="G86" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H86">
         <v>0</v>
       </c>
@@ -3351,6 +3614,9 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
+      <c r="G87" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H87">
         <v>0</v>
       </c>
@@ -3378,6 +3644,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="G88" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H88">
         <v>-2.5</v>
       </c>
@@ -3405,6 +3674,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="G89" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H89">
         <v>-2.5</v>
       </c>
@@ -3432,6 +3704,9 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="G90" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H90">
         <v>0</v>
       </c>
@@ -3459,6 +3734,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="G91" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H91">
         <v>0</v>
       </c>
@@ -3486,6 +3764,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="G92" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H92">
         <v>0</v>
       </c>
@@ -3513,6 +3794,9 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="G93" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H93">
         <v>0</v>
       </c>
@@ -3520,7 +3804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>99</v>
       </c>
@@ -3540,6 +3824,9 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="G94">
+        <v>1000</v>
+      </c>
       <c r="H94">
         <v>0</v>
       </c>
@@ -3567,6 +3854,9 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
+      <c r="G95" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H95">
         <v>0</v>
       </c>
@@ -3594,6 +3884,9 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
+      <c r="G96" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H96">
         <v>0</v>
       </c>
@@ -3621,6 +3914,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="G97" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H97">
         <v>0</v>
       </c>
@@ -3628,7 +3924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>104</v>
       </c>
@@ -3648,11 +3944,14 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="G98">
+        <v>1000</v>
+      </c>
       <c r="H98">
         <v>0</v>
       </c>
       <c r="I98">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -3675,6 +3974,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="G99" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H99">
         <v>0</v>
       </c>
@@ -3682,7 +3984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>106</v>
       </c>
@@ -3701,6 +4003,9 @@
       <c r="F100">
         <f t="shared" si="1"/>
         <v>5</v>
+      </c>
+      <c r="G100">
+        <v>1000</v>
       </c>
       <c r="H100">
         <v>0</v>
@@ -3729,6 +4034,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="G101" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H101">
         <v>0</v>
       </c>
@@ -3756,6 +4064,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="G102" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H102">
         <v>0</v>
       </c>
@@ -3783,6 +4094,9 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
+      <c r="G103" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H103">
         <v>0</v>
       </c>
@@ -3790,7 +4104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>110</v>
       </c>
@@ -3810,6 +4124,9 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="G104">
+        <v>1000</v>
+      </c>
       <c r="H104">
         <v>0</v>
       </c>
@@ -3837,6 +4154,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="G105" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H105">
         <v>0</v>
       </c>
@@ -3849,7 +4169,7 @@
         <v>113</v>
       </c>
       <c r="B106">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C106">
         <v>100</v>
@@ -3864,6 +4184,9 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
+      <c r="G106" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H106">
         <v>0</v>
       </c>
@@ -3891,6 +4214,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="G107" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H107">
         <v>-3.5</v>
       </c>
@@ -3918,6 +4244,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="G108" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H108">
         <v>-5.5</v>
       </c>
@@ -3925,7 +4254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>116</v>
       </c>
@@ -3945,6 +4274,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="G109">
+        <v>1000</v>
+      </c>
       <c r="H109">
         <v>-5.5</v>
       </c>
@@ -3972,6 +4304,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="G110" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H110">
         <v>0</v>
       </c>
@@ -3999,6 +4334,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="G111" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H111">
         <v>0</v>
       </c>
@@ -4026,6 +4364,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="G112" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H112">
         <v>0</v>
       </c>
@@ -4053,6 +4394,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="G113" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H113">
         <v>-2.5</v>
       </c>
@@ -4080,6 +4424,9 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="G114" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H114">
         <v>0</v>
       </c>
@@ -4107,6 +4454,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="G115" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H115">
         <v>-1.5</v>
       </c>
@@ -4134,6 +4484,9 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="G116" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H116">
         <v>0</v>
       </c>
@@ -4161,6 +4514,9 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
+      <c r="G117" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H117">
         <v>0</v>
       </c>
@@ -4188,6 +4544,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="G118" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H118">
         <v>0</v>
       </c>
@@ -4215,6 +4574,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="G119" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H119">
         <v>0</v>
       </c>
@@ -4242,6 +4604,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="G120" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H120">
         <v>-3.5</v>
       </c>
@@ -4269,6 +4634,9 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
+      <c r="G121" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H121">
         <v>0</v>
       </c>
@@ -4296,6 +4664,9 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
+      <c r="G122" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H122">
         <v>0</v>
       </c>
@@ -4323,6 +4694,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="G123" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H123">
         <v>-3</v>
       </c>
@@ -4350,6 +4724,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="G124" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H124">
         <v>0</v>
       </c>
@@ -4357,7 +4734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>133</v>
       </c>
@@ -4376,6 +4753,9 @@
       <c r="F125">
         <f t="shared" si="1"/>
         <v>5</v>
+      </c>
+      <c r="G125">
+        <v>1000</v>
       </c>
       <c r="H125">
         <v>1.25</v>
@@ -4404,6 +4784,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
+      <c r="G126" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H126">
         <v>0</v>
       </c>
@@ -4431,6 +4814,9 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
+      <c r="G127" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H127">
         <v>0</v>
       </c>
@@ -4438,7 +4824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>137</v>
       </c>
@@ -4458,6 +4844,9 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
+      <c r="G128">
+        <v>1000</v>
+      </c>
       <c r="H128">
         <v>2</v>
       </c>
@@ -4485,6 +4874,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="G129" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H129">
         <v>0</v>
       </c>
@@ -4512,6 +4904,9 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
+      <c r="G130" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H130">
         <v>0</v>
       </c>
@@ -4539,6 +4934,9 @@
         <f t="shared" ref="F131:F184" si="2">ROUND(D131,0)</f>
         <v>8</v>
       </c>
+      <c r="G131" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H131">
         <v>0</v>
       </c>
@@ -4551,7 +4949,7 @@
         <v>141</v>
       </c>
       <c r="B132">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C132">
         <v>100</v>
@@ -4566,6 +4964,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
+      <c r="G132" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H132">
         <v>0</v>
       </c>
@@ -4593,6 +4994,9 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
+      <c r="G133" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H133">
         <v>0</v>
       </c>
@@ -4620,6 +5024,9 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
+      <c r="G134" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H134">
         <v>0</v>
       </c>
@@ -4647,6 +5054,9 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
+      <c r="G135" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H135">
         <v>-2.5</v>
       </c>
@@ -4654,7 +5064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>146</v>
       </c>
@@ -4673,6 +5083,9 @@
       <c r="F136">
         <f t="shared" si="2"/>
         <v>10</v>
+      </c>
+      <c r="G136">
+        <v>1000</v>
       </c>
       <c r="H136">
         <v>2.25</v>
@@ -4701,6 +5114,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
+      <c r="G137" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H137">
         <v>0</v>
       </c>
@@ -4728,6 +5144,9 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
+      <c r="G138" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H138">
         <v>0</v>
       </c>
@@ -4755,6 +5174,9 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
+      <c r="G139" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H139">
         <v>0</v>
       </c>
@@ -4782,6 +5204,9 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
+      <c r="G140" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H140">
         <v>0</v>
       </c>
@@ -4809,6 +5234,9 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
+      <c r="G141" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H141">
         <v>0</v>
       </c>
@@ -4816,7 +5244,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>152</v>
       </c>
@@ -4836,6 +5264,9 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
+      <c r="G142">
+        <v>1000</v>
+      </c>
       <c r="H142">
         <v>0</v>
       </c>
@@ -4843,7 +5274,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>153</v>
       </c>
@@ -4863,6 +5294,9 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
+      <c r="G143">
+        <v>1000</v>
+      </c>
       <c r="H143">
         <v>0</v>
       </c>
@@ -4890,6 +5324,9 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
+      <c r="G144" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H144">
         <v>0</v>
       </c>
@@ -4897,7 +5334,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>155</v>
       </c>
@@ -4917,6 +5354,9 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
+      <c r="G145">
+        <v>1000</v>
+      </c>
       <c r="H145">
         <v>3.25</v>
       </c>
@@ -4944,6 +5384,9 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
+      <c r="G146" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H146">
         <v>0</v>
       </c>
@@ -4956,7 +5399,7 @@
         <v>158</v>
       </c>
       <c r="B147">
-        <v>-60</v>
+        <v>60</v>
       </c>
       <c r="C147">
         <v>100</v>
@@ -4970,6 +5413,9 @@
       <c r="F147">
         <f t="shared" si="2"/>
         <v>5</v>
+      </c>
+      <c r="G147" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="H147">
         <v>0</v>
@@ -4998,6 +5444,9 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
+      <c r="G148" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H148">
         <v>0</v>
       </c>
@@ -5025,6 +5474,9 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
+      <c r="G149" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H149">
         <v>-2.5</v>
       </c>
@@ -5052,6 +5504,9 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
+      <c r="G150" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H150">
         <v>-1.25</v>
       </c>
@@ -5079,6 +5534,9 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
+      <c r="G151" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H151">
         <v>0</v>
       </c>
@@ -5086,7 +5544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>163</v>
       </c>
@@ -5106,6 +5564,9 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
+      <c r="G152">
+        <v>1000</v>
+      </c>
       <c r="H152">
         <v>1</v>
       </c>
@@ -5113,7 +5574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>164</v>
       </c>
@@ -5133,6 +5594,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
+      <c r="G153">
+        <v>1000</v>
+      </c>
       <c r="H153">
         <v>-5.5</v>
       </c>
@@ -5160,6 +5624,9 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
+      <c r="G154" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H154">
         <v>0</v>
       </c>
@@ -5187,6 +5654,9 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
+      <c r="G155" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H155">
         <v>4</v>
       </c>
@@ -5214,6 +5684,9 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
+      <c r="G156" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H156">
         <v>0</v>
       </c>
@@ -5241,6 +5714,9 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
+      <c r="G157" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H157">
         <v>0</v>
       </c>
@@ -5268,6 +5744,9 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
+      <c r="G158" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H158">
         <v>0</v>
       </c>
@@ -5295,6 +5774,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
+      <c r="G159" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H159">
         <v>0</v>
       </c>
@@ -5302,7 +5784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>172</v>
       </c>
@@ -5321,6 +5803,9 @@
       <c r="F160">
         <f t="shared" si="2"/>
         <v>10</v>
+      </c>
+      <c r="G160">
+        <v>1000</v>
       </c>
       <c r="H160">
         <v>3.25</v>
@@ -5349,6 +5834,9 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
+      <c r="G161" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H161">
         <v>0</v>
       </c>
@@ -5376,6 +5864,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
+      <c r="G162" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H162">
         <v>-3.5</v>
       </c>
@@ -5403,6 +5894,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
+      <c r="G163" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H163">
         <v>0</v>
       </c>
@@ -5430,6 +5924,9 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
+      <c r="G164" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H164">
         <v>0</v>
       </c>
@@ -5437,7 +5934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>177</v>
       </c>
@@ -5457,6 +5954,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
+      <c r="G165">
+        <v>1000</v>
+      </c>
       <c r="H165">
         <v>2.25</v>
       </c>
@@ -5484,6 +5984,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
+      <c r="G166" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H166">
         <v>-2.5</v>
       </c>
@@ -5511,6 +6014,9 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
+      <c r="G167" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H167">
         <v>1</v>
       </c>
@@ -5538,6 +6044,9 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
+      <c r="G168" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H168">
         <v>2</v>
       </c>
@@ -5565,6 +6074,9 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
+      <c r="G169" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H169">
         <v>0</v>
       </c>
@@ -5592,6 +6104,9 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
+      <c r="G170" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H170">
         <v>0</v>
       </c>
@@ -5619,6 +6134,9 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
+      <c r="G171" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H171">
         <v>1</v>
       </c>
@@ -5646,6 +6164,9 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
+      <c r="G172" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H172">
         <v>0</v>
       </c>
@@ -5673,6 +6194,9 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
+      <c r="G173" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H173">
         <v>0</v>
       </c>
@@ -5680,7 +6204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>187</v>
       </c>
@@ -5700,6 +6224,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
+      <c r="G174">
+        <v>1000</v>
+      </c>
       <c r="H174">
         <v>3.25</v>
       </c>
@@ -5727,6 +6254,9 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
+      <c r="G175" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H175">
         <v>-3.5</v>
       </c>
@@ -5754,6 +6284,9 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
+      <c r="G176" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H176">
         <v>-3.5</v>
       </c>
@@ -5781,6 +6314,9 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
+      <c r="G177" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H177">
         <v>0</v>
       </c>
@@ -5808,6 +6344,9 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
+      <c r="G178" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H178">
         <v>0</v>
       </c>
@@ -5835,6 +6374,9 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
+      <c r="G179" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H179">
         <v>-5.5</v>
       </c>
@@ -5862,6 +6404,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
+      <c r="G180" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H180">
         <v>0</v>
       </c>
@@ -5889,6 +6434,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
+      <c r="G181" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H181">
         <v>0</v>
       </c>
@@ -5916,6 +6464,9 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
+      <c r="G182" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H182">
         <v>0</v>
       </c>
@@ -5923,7 +6474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>197</v>
       </c>
@@ -5943,6 +6494,9 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
+      <c r="G183">
+        <v>1000</v>
+      </c>
       <c r="H183">
         <v>2</v>
       </c>
@@ -5970,6 +6524,9 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
+      <c r="G184" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="H184">
         <v>0</v>
       </c>
@@ -5978,6 +6535,36 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I184">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="1"/>
+        <filter val="10"/>
+        <filter val="100"/>
+        <filter val="10000"/>
+        <filter val="110"/>
+        <filter val="120"/>
+        <filter val="130"/>
+        <filter val="140"/>
+        <filter val="15"/>
+        <filter val="150"/>
+        <filter val="20"/>
+        <filter val="25"/>
+        <filter val="30"/>
+        <filter val="40"/>
+        <filter val="50"/>
+        <filter val="55"/>
+        <filter val="60"/>
+        <filter val="65"/>
+        <filter val="70"/>
+        <filter val="75"/>
+        <filter val="80"/>
+        <filter val="85"/>
+        <filter val="90"/>
+        <filter val="95"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated ice ball like moves, confusion/paralysis not working
</commit_message>
<xml_diff>
--- a/moves.xlsx
+++ b/moves.xlsx
@@ -1001,8 +1001,8 @@
   <dimension ref="A1:J184"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,7 +1096,7 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:G66" si="0">ROUND(D3,0)</f>
+        <f t="shared" ref="F3:F66" si="0">ROUND(D3,0)</f>
         <v>5</v>
       </c>
       <c r="G3" s="1">
@@ -1117,7 +1117,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>95</v>

</xml_diff>